<commit_message>
Template du site + mld mcd + arborescence du site
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord TPI.xlsx
+++ b/Documentation/Journal de bord TPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -69,6 +69,33 @@
   </si>
   <si>
     <t>Preparation du mail d'envoie</t>
+  </si>
+  <si>
+    <t>MCD numerique</t>
+  </si>
+  <si>
+    <t>MLD numerique</t>
+  </si>
+  <si>
+    <t>MCD-MLD papier</t>
+  </si>
+  <si>
+    <t>Preparation du template / maquette visuel</t>
+  </si>
+  <si>
+    <t>Utilisation d'un logiciel nommé nicepage pour crée un template. Il me faut demander a mon chef de projet si il considere ok pour une maquette visuel</t>
+  </si>
+  <si>
+    <t>Arborescence du site</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>MCD-MLD decrit + mise en page + premier point de la docs ecrit</t>
+  </si>
+  <si>
+    <t>Planification initiale</t>
   </si>
 </sst>
 </file>
@@ -741,7 +768,7 @@
   <dimension ref="B1:E82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +847,9 @@
       <c r="D6" s="10">
         <v>120</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
@@ -849,40 +878,80 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="19"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
+      <c r="B9" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="9">
+        <v>44320</v>
+      </c>
+      <c r="D9" s="10">
+        <v>40</v>
+      </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10"/>
+      <c r="B10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="9">
+        <v>44320</v>
+      </c>
+      <c r="D10" s="10">
+        <v>25</v>
+      </c>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="19"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
+      <c r="B11" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="9">
+        <v>44320</v>
+      </c>
+      <c r="D11" s="10">
+        <v>60</v>
+      </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="19"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="5"/>
+    <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="9">
+        <v>44320</v>
+      </c>
+      <c r="D12" s="10">
+        <v>120</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
+      <c r="B13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="9">
+        <v>44320</v>
+      </c>
+      <c r="D13" s="10">
+        <v>40</v>
+      </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="19"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="5"/>
+      <c r="B14" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="9">
+        <v>44320</v>
+      </c>
+      <c r="D14" s="10">
+        <v>120</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="19"/>

</xml_diff>

<commit_message>
Toutes les maquettes graphique
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord TPI.xlsx
+++ b/Documentation/Journal de bord TPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -92,10 +92,34 @@
     <t>Documentation</t>
   </si>
   <si>
-    <t>MCD-MLD decrit + mise en page + premier point de la docs ecrit</t>
-  </si>
-  <si>
     <t>Planification initiale</t>
+  </si>
+  <si>
+    <t>Documentation de mon mcd-mld</t>
+  </si>
+  <si>
+    <t>Mise en page + premier point de la docs ecrit</t>
+  </si>
+  <si>
+    <t>Ecriture des points dans la docs de chaque tables des mcd-mld</t>
+  </si>
+  <si>
+    <t>Création de la maquettes visuel de tout le site</t>
+  </si>
+  <si>
+    <t>Ecriture du mail d'envoie des PDF</t>
+  </si>
+  <si>
+    <t>Comme demandé par Monsieur Montemayor, un envoie au format PDF de la documentation et du journal de travail. J'ai vite remis en forme un bug sur la doc</t>
+  </si>
+  <si>
+    <t>Cela m'a pris pas mal de temps, J'ai fais les maquettes pour l'acceuil, Mon calendrier vue mois et semaine, modifier/ajouter évènement, contact, login, register, profil</t>
+  </si>
+  <si>
+    <t>Discussion avec le chef de projet</t>
+  </si>
+  <si>
+    <t>A propos de la pertinance d'un gantt dans un projet en mode Agile. Resultat: Pas besoin j'ai fais juste.</t>
   </si>
 </sst>
 </file>
@@ -290,14 +314,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -351,6 +372,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -767,8 +794,8 @@
   </sheetPr>
   <dimension ref="B1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E23" sqref="E22:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,568 +825,600 @@
       </c>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>44319</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>45</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="23" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>44319</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>45</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="22" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>44319</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>60</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="22"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>44319</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>120</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="8">
+        <v>44319</v>
+      </c>
+      <c r="D7" s="9">
+        <v>60</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="8">
+        <v>44319</v>
+      </c>
+      <c r="D8" s="9">
+        <v>60</v>
+      </c>
+      <c r="E8" s="22"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="8">
+        <v>44320</v>
+      </c>
+      <c r="D9" s="9">
+        <v>40</v>
+      </c>
+      <c r="E9" s="22"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="8">
+        <v>44320</v>
+      </c>
+      <c r="D10" s="9">
+        <v>25</v>
+      </c>
+      <c r="E10" s="22"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="8">
+        <v>44320</v>
+      </c>
+      <c r="D11" s="9">
+        <v>60</v>
+      </c>
+      <c r="E11" s="22"/>
+    </row>
+    <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="8">
+        <v>44320</v>
+      </c>
+      <c r="D12" s="9">
+        <v>120</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="8">
+        <v>44320</v>
+      </c>
+      <c r="D13" s="9">
+        <v>40</v>
+      </c>
+      <c r="E13" s="22"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="8">
+        <v>44320</v>
+      </c>
+      <c r="D14" s="9">
+        <v>120</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="9">
-        <v>44319</v>
-      </c>
-      <c r="D7" s="10">
-        <v>60</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="9">
-        <v>44319</v>
-      </c>
-      <c r="D8" s="10">
-        <v>60</v>
-      </c>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
+      <c r="C15" s="8">
+        <v>44320</v>
+      </c>
+      <c r="D15" s="9">
+        <v>40</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="8">
+        <v>44322</v>
+      </c>
+      <c r="D16" s="9">
         <v>15</v>
       </c>
-      <c r="C9" s="9">
-        <v>44320</v>
-      </c>
-      <c r="D9" s="10">
-        <v>40</v>
-      </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="9">
-        <v>44320</v>
-      </c>
-      <c r="D10" s="10">
-        <v>25</v>
-      </c>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="9">
-        <v>44320</v>
-      </c>
-      <c r="D11" s="10">
-        <v>60</v>
-      </c>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="9">
-        <v>44320</v>
-      </c>
-      <c r="D12" s="10">
-        <v>120</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="9">
-        <v>44320</v>
-      </c>
-      <c r="D13" s="10">
-        <v>40</v>
-      </c>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="9">
-        <v>44320</v>
-      </c>
-      <c r="D14" s="10">
-        <v>120</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="19"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="19"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="5"/>
+      <c r="E16" s="22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B17" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="8">
+        <v>44322</v>
+      </c>
+      <c r="D17" s="9">
+        <v>180</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="8">
+        <v>44322</v>
+      </c>
+      <c r="D18" s="9">
+        <v>10</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="19"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="5"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="22"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="5"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="22"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="19"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="5"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="22"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="5"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="22"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="19"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="5"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="22"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="19"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="5"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="22"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="19"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="5"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="22"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="5"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="22"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="19"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="5"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="22"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="19"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="5"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="22"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="19"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="5"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="22"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="19"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="5"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="22"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="19"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="5"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="22"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="5"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="22"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="19"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="5"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="22"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="19"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="5"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="22"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="19"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="5"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="22"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="19"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="5"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="22"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="19"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="5"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="22"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="19"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="5"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="22"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="19"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="5"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="22"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="8"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="5"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="22"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="8"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="5"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="22"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="19"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="5"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="22"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="19"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="5"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="22"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="19"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="5"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="22"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="19"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="5"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="22"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="19"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="5"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="22"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="19"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="5"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="22"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="19"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="5"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="22"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="19"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="5"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="22"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="19"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="5"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="22"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="19"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="5"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="22"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="19"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="5"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="22"/>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="19"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="21"/>
-      <c r="E53" s="5"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="22"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="19"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="21"/>
-      <c r="E54" s="5"/>
+      <c r="B54" s="18"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="22"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="19"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="21"/>
-      <c r="E55" s="5"/>
+      <c r="B55" s="18"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="22"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="19"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="5"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="22"/>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="19"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="5"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="22"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="19"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="5"/>
+      <c r="B58" s="18"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="22"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="19"/>
-      <c r="C59" s="20"/>
-      <c r="D59" s="21"/>
-      <c r="E59" s="5"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="22"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="19"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="21"/>
-      <c r="E60" s="5"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="22"/>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="19"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="21"/>
-      <c r="E61" s="5"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="22"/>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="19"/>
-      <c r="C62" s="20"/>
-      <c r="D62" s="21"/>
-      <c r="E62" s="5"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="22"/>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="19"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="21"/>
-      <c r="E63" s="5"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="22"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="19"/>
-      <c r="C64" s="20"/>
-      <c r="D64" s="21"/>
-      <c r="E64" s="5"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="19"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="22"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="19"/>
-      <c r="C65" s="20"/>
-      <c r="D65" s="21"/>
-      <c r="E65" s="5"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="22"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="19"/>
-      <c r="C66" s="20"/>
-      <c r="D66" s="21"/>
-      <c r="E66" s="5"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="22"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="19"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="21"/>
-      <c r="E67" s="5"/>
+      <c r="B67" s="18"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="22"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="19"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="21"/>
-      <c r="E68" s="5"/>
+      <c r="B68" s="18"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="22"/>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="19"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="21"/>
-      <c r="E69" s="5"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="22"/>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="19"/>
-      <c r="C70" s="20"/>
-      <c r="D70" s="21"/>
-      <c r="E70" s="5"/>
+      <c r="B70" s="18"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="22"/>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B71" s="19"/>
-      <c r="C71" s="20"/>
-      <c r="D71" s="21"/>
-      <c r="E71" s="5"/>
+      <c r="B71" s="18"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="22"/>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="19"/>
-      <c r="C72" s="20"/>
-      <c r="D72" s="21"/>
-      <c r="E72" s="5"/>
+      <c r="B72" s="18"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="22"/>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="19"/>
-      <c r="C73" s="20"/>
-      <c r="D73" s="21"/>
-      <c r="E73" s="5"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="22"/>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B74" s="19"/>
-      <c r="C74" s="20"/>
-      <c r="D74" s="21"/>
-      <c r="E74" s="5"/>
+      <c r="B74" s="18"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="22"/>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B75" s="19"/>
-      <c r="C75" s="20"/>
-      <c r="D75" s="21"/>
-      <c r="E75" s="5"/>
+      <c r="B75" s="18"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="22"/>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B76" s="19"/>
-      <c r="C76" s="20"/>
-      <c r="D76" s="21"/>
-      <c r="E76" s="5"/>
+      <c r="B76" s="18"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="22"/>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B77" s="19"/>
-      <c r="C77" s="20"/>
-      <c r="D77" s="21"/>
-      <c r="E77" s="5"/>
+      <c r="B77" s="18"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="20"/>
+      <c r="E77" s="22"/>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="19"/>
-      <c r="C78" s="20"/>
-      <c r="D78" s="21"/>
-      <c r="E78" s="5"/>
+      <c r="B78" s="18"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="22"/>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B79" s="19"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="21"/>
-      <c r="E79" s="5"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="20"/>
+      <c r="E79" s="4"/>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="19"/>
-      <c r="C80" s="20"/>
-      <c r="D80" s="21"/>
-      <c r="E80" s="5"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="4"/>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="22"/>
-      <c r="C81" s="22"/>
-      <c r="D81" s="22"/>
-      <c r="E81" s="22"/>
+      <c r="B81" s="21"/>
+      <c r="C81" s="21"/>
+      <c r="D81" s="21"/>
+      <c r="E81" s="21"/>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B82" s="13"/>
-      <c r="C82" s="14"/>
-      <c r="D82" s="15"/>
-      <c r="E82" s="16"/>
+      <c r="B82" s="12"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Retouche de 2-3 maquette + documentation avec maquette
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord TPI.xlsx
+++ b/Documentation/Journal de bord TPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>A propos de la pertinance d'un gantt dans un projet en mode Agile. Resultat: Pas besoin j'ai fais juste.</t>
+  </si>
+  <si>
+    <t>Ajout des maquettes et commentaires dans la documentation</t>
+  </si>
+  <si>
+    <t>Debut de usercase + test</t>
   </si>
 </sst>
 </file>
@@ -794,8 +800,8 @@
   </sheetPr>
   <dimension ref="B1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E23" sqref="E22:E23"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,17 +1042,29 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="18"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
+    <row r="19" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="8">
+        <v>44322</v>
+      </c>
+      <c r="D19" s="9">
+        <v>60</v>
+      </c>
       <c r="E19" s="22"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="18"/>
+      <c r="B20" s="18" t="s">
+        <v>19</v>
+      </c>
       <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="22"/>
+      <c r="D20" s="9">
+        <v>120</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="18"/>

</xml_diff>

<commit_message>
Update du journal de bord
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord TPI.xlsx
+++ b/Documentation/Journal de bord TPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -125,13 +125,40 @@
     <t>Ajout des maquettes et commentaires dans la documentation</t>
   </si>
   <si>
-    <t>Debut de usercase + test</t>
-  </si>
-  <si>
     <t>Derniere retouche sur les maquettes graphique</t>
   </si>
   <si>
     <t>2-3 mots a passer d'anglais a français + bug d'affichage</t>
+  </si>
+  <si>
+    <t>Recherche a propos du code du calendrier</t>
+  </si>
+  <si>
+    <t>Etant donné que j'ai fini le sprint 1, je me documente déjà sur comment va se passer la suite histoire de me donné une idée de combien de temps cela va prendre. J'ai déjà reussi a trouver un code source a étudier: https://codes-sources.commentcamarche.net/source/50541-calendrier-agenda-tres-simple-gerer-les-jours-feries-et-les-jours-speciaux</t>
+  </si>
+  <si>
+    <t>Ajout d'un ReadMe sur le Git</t>
+  </si>
+  <si>
+    <t>Ajout + ecritude de celui-ci + redecouverte du MarkDown</t>
+  </si>
+  <si>
+    <t>Retrospective Sprint 1 sur le Git</t>
+  </si>
+  <si>
+    <t>en + passage du git en public, sinon la creation d'un git n'est pas possible</t>
+  </si>
+  <si>
+    <t>Debut de usercase + test + autres points de la doc de l'analyse et conception</t>
+  </si>
+  <si>
+    <t>Debut du touchage de code avec le calendrier</t>
+  </si>
+  <si>
+    <t>En attendant la fin du sprint qui est la fin de cette journée.</t>
+  </si>
+  <si>
+    <t>En attendant la fin du sprint qui est la fin de cette journée. Couleur du calendrier, test des fonctionalité, design, etc. Pas de code majeur juste de la mise en page.</t>
   </si>
 </sst>
 </file>
@@ -807,7 +834,7 @@
   <dimension ref="B1:E82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,12 +1098,12 @@
         <v>120</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="8">
         <v>44322</v>
@@ -1085,32 +1112,64 @@
         <v>60</v>
       </c>
       <c r="E21" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B22" s="18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="18"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="22"/>
+      <c r="C22" s="8">
+        <v>44323</v>
+      </c>
+      <c r="D22" s="9">
+        <v>60</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="18"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="22"/>
+      <c r="B23" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="8">
+        <v>44323</v>
+      </c>
+      <c r="D23" s="9">
+        <v>30</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="18"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="22"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="18"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="22"/>
+      <c r="B24" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="8">
+        <v>44323</v>
+      </c>
+      <c r="D24" s="9">
+        <v>60</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B25" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="8">
+        <v>44323</v>
+      </c>
+      <c r="D25" s="9">
+        <v>60</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="18"/>

</xml_diff>

<commit_message>
Structure MVC + Diagram code + SQL
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord TPI.xlsx
+++ b/Documentation/Journal de bord TPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>Date</t>
   </si>
@@ -47,27 +47,18 @@
     <t>Lecture du CDC avec les experts</t>
   </si>
   <si>
-    <t>Reçu le cahier des charges + premier entretient avec Monsieur Montemayor</t>
-  </si>
-  <si>
     <t>Creation du Git + IceScrum</t>
   </si>
   <si>
     <t>Sprints + tasks IceScrum</t>
   </si>
   <si>
-    <t>Prise en main de icescrum</t>
-  </si>
-  <si>
     <t>Creation des premiers documents</t>
   </si>
   <si>
     <t>Realisation des sprints sur papier</t>
   </si>
   <si>
-    <t>Plus debut de la mise en page de la Doc</t>
-  </si>
-  <si>
     <t>Preparation du mail d'envoie</t>
   </si>
   <si>
@@ -83,36 +74,21 @@
     <t>Preparation du template / maquette visuel</t>
   </si>
   <si>
-    <t>Utilisation d'un logiciel nommé nicepage pour crée un template. Il me faut demander a mon chef de projet si il considere ok pour une maquette visuel</t>
-  </si>
-  <si>
     <t>Arborescence du site</t>
   </si>
   <si>
     <t>Documentation</t>
   </si>
   <si>
-    <t>Planification initiale</t>
-  </si>
-  <si>
     <t>Documentation de mon mcd-mld</t>
   </si>
   <si>
-    <t>Mise en page + premier point de la docs ecrit</t>
-  </si>
-  <si>
-    <t>Ecriture des points dans la docs de chaque tables des mcd-mld</t>
-  </si>
-  <si>
     <t>Création de la maquettes visuel de tout le site</t>
   </si>
   <si>
     <t>Ecriture du mail d'envoie des PDF</t>
   </si>
   <si>
-    <t>Comme demandé par Monsieur Montemayor, un envoie au format PDF de la documentation et du journal de travail. J'ai vite remis en forme un bug sur la doc</t>
-  </si>
-  <si>
     <t>Cela m'a pris pas mal de temps, J'ai fais les maquettes pour l'acceuil, Mon calendrier vue mois et semaine, modifier/ajouter évènement, contact, login, register, profil</t>
   </si>
   <si>
@@ -128,9 +104,6 @@
     <t>Derniere retouche sur les maquettes graphique</t>
   </si>
   <si>
-    <t>2-3 mots a passer d'anglais a français + bug d'affichage</t>
-  </si>
-  <si>
     <t>Recherche a propos du code du calendrier</t>
   </si>
   <si>
@@ -140,25 +113,79 @@
     <t>Ajout d'un ReadMe sur le Git</t>
   </si>
   <si>
-    <t>Ajout + ecritude de celui-ci + redecouverte du MarkDown</t>
-  </si>
-  <si>
     <t>Retrospective Sprint 1 sur le Git</t>
   </si>
   <si>
-    <t>en + passage du git en public, sinon la creation d'un git n'est pas possible</t>
-  </si>
-  <si>
-    <t>Debut de usercase + test + autres points de la doc de l'analyse et conception</t>
-  </si>
-  <si>
     <t>Debut du touchage de code avec le calendrier</t>
   </si>
   <si>
-    <t>En attendant la fin du sprint qui est la fin de cette journée.</t>
-  </si>
-  <si>
     <t>En attendant la fin du sprint qui est la fin de cette journée. Couleur du calendrier, test des fonctionalité, design, etc. Pas de code majeur juste de la mise en page.</t>
+  </si>
+  <si>
+    <t>Ecriture des test et taches du sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 1 review</t>
+  </si>
+  <si>
+    <t>Création de la base de donnée</t>
+  </si>
+  <si>
+    <t>Architecture MVC</t>
+  </si>
+  <si>
+    <t>Adaptation du Template en MVC + Redirection pour une navigation basique sur le site.</t>
+  </si>
+  <si>
+    <t>Modification dans la doc</t>
+  </si>
+  <si>
+    <t>Les modifications sont en rapport a ce d'ont nous avons parler pendant la sprint review.</t>
+  </si>
+  <si>
+    <t>Ajout + ecritude de celui-ci + redecouverte du MarkDown.</t>
+  </si>
+  <si>
+    <t>en + passage du git en public, sinon la creation d'un git n'est pas possible.</t>
+  </si>
+  <si>
+    <t>Comme demandé par Monsieur Montemayor, un envoie au format PDF de la documentation et du journal de travail. J'ai vite remis en forme un bug sur la doc.</t>
+  </si>
+  <si>
+    <t>Ecriture des points dans la docs de chaque tables des mcd-mld.</t>
+  </si>
+  <si>
+    <t>Mise en page + premier point de la docs ecrit.</t>
+  </si>
+  <si>
+    <t>Utilisation d'un logiciel nommé nicepage pour crée un template. Il me faut demander a mon chef de projet si il considere ok pour une maquette visuel.</t>
+  </si>
+  <si>
+    <t>Plus debut de la mise en page de la Doc.</t>
+  </si>
+  <si>
+    <t>Planification initiale.</t>
+  </si>
+  <si>
+    <t>Prise en main de icescrum.</t>
+  </si>
+  <si>
+    <t>Reçu le cahier des charges + premier entretient avec Monsieur Montemayor.</t>
+  </si>
+  <si>
+    <t>Debut de usercase + test + autres points de la doc de l'analyse et conception.</t>
+  </si>
+  <si>
+    <t>2-3 mots a passer d'anglais a français + bug d'affichage.</t>
+  </si>
+  <si>
+    <t>Base de donnée + utilisateur.</t>
+  </si>
+  <si>
+    <t>Diagramme de code pour ajouter un évènement</t>
+  </si>
+  <si>
+    <t>Charte graphique + 2-3 autres points</t>
   </si>
 </sst>
 </file>
@@ -833,8 +860,8 @@
   </sheetPr>
   <dimension ref="B1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,12 +901,12 @@
         <v>45</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="10">
         <v>44319</v>
@@ -888,12 +915,12 @@
         <v>45</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="8">
         <v>44319</v>
@@ -905,7 +932,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="8">
         <v>44319</v>
@@ -914,12 +941,12 @@
         <v>120</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="8">
         <v>44319</v>
@@ -928,12 +955,12 @@
         <v>60</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C8" s="8">
         <v>44319</v>
@@ -945,7 +972,7 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C9" s="8">
         <v>44320</v>
@@ -957,7 +984,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C10" s="8">
         <v>44320</v>
@@ -969,7 +996,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C11" s="8">
         <v>44320</v>
@@ -981,7 +1008,7 @@
     </row>
     <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C12" s="8">
         <v>44320</v>
@@ -990,12 +1017,12 @@
         <v>120</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C13" s="8">
         <v>44320</v>
@@ -1007,7 +1034,7 @@
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C14" s="8">
         <v>44320</v>
@@ -1016,12 +1043,12 @@
         <v>120</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C15" s="8">
         <v>44320</v>
@@ -1030,12 +1057,12 @@
         <v>40</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="7" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C16" s="8">
         <v>44322</v>
@@ -1044,12 +1071,12 @@
         <v>15</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C17" s="8">
         <v>44322</v>
@@ -1058,12 +1085,12 @@
         <v>180</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C18" s="8">
         <v>44322</v>
@@ -1072,12 +1099,12 @@
         <v>10</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C19" s="8">
         <v>44322</v>
@@ -1089,7 +1116,7 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C20" s="8">
         <v>44322</v>
@@ -1098,12 +1125,12 @@
         <v>120</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C21" s="8">
         <v>44322</v>
@@ -1112,12 +1139,12 @@
         <v>60</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B22" s="18" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C22" s="8">
         <v>44323</v>
@@ -1126,12 +1153,12 @@
         <v>60</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="18" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C23" s="8">
         <v>44323</v>
@@ -1140,12 +1167,12 @@
         <v>30</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C24" s="8">
         <v>44323</v>
@@ -1159,7 +1186,7 @@
     </row>
     <row r="25" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C25" s="8">
         <v>44323</v>
@@ -1168,50 +1195,100 @@
         <v>60</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="18"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
+      <c r="B26" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="8">
+        <v>44326</v>
+      </c>
+      <c r="D26" s="9">
+        <v>60</v>
+      </c>
       <c r="E26" s="22"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="18"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
+      <c r="B27" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="8">
+        <v>44326</v>
+      </c>
+      <c r="D27" s="9">
+        <v>60</v>
+      </c>
       <c r="E27" s="22"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="18"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="22"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="18"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="22"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="18"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="22"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="18"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
+      <c r="B28" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="8">
+        <v>44326</v>
+      </c>
+      <c r="D28" s="9">
+        <v>30</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="8">
+        <v>44326</v>
+      </c>
+      <c r="D29" s="9">
+        <v>60</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="8">
+        <v>44326</v>
+      </c>
+      <c r="D30" s="9">
+        <v>120</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="8">
+        <v>44326</v>
+      </c>
+      <c r="D31" s="9">
+        <v>60</v>
+      </c>
       <c r="E31" s="22"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="22"/>
+      <c r="B32" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="8">
+        <v>44326</v>
+      </c>
+      <c r="D32" s="9">
+        <v>30</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="18"/>

</xml_diff>

<commit_message>
Diagram updated + debut du login
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord TPI.xlsx
+++ b/Documentation/Journal de bord TPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
   <si>
     <t>Date</t>
   </si>
@@ -186,6 +186,51 @@
   </si>
   <si>
     <t>Charte graphique + 2-3 autres points</t>
+  </si>
+  <si>
+    <t>Diagramme de code pour modifier un évènement</t>
+  </si>
+  <si>
+    <t>Diagramme de code pour supprimer un évènement</t>
+  </si>
+  <si>
+    <t>Modification de 2-3 trucs</t>
+  </si>
+  <si>
+    <t>Reprise du debut de code du calendrier et mise a niveau des couleurs avec la charte graphique de la doc</t>
+  </si>
+  <si>
+    <t>Couleur + petite adaptation aux besoins</t>
+  </si>
+  <si>
+    <t>Mise en place de l'hebergement</t>
+  </si>
+  <si>
+    <t>Discussion avec le chef de projet + ajout du site vitrine sur swisscenter</t>
+  </si>
+  <si>
+    <t>Ajout des diagramme dans la documentation</t>
+  </si>
+  <si>
+    <t>Travail sur l'ajout d'un login pour le site vitrine</t>
+  </si>
+  <si>
+    <t>Pas encore au points a cause de tout ce qu'il faut retoucher. Ex: name des label du template, redirection, etc..</t>
+  </si>
+  <si>
+    <t>Sprint 2 fini a partir d'ici</t>
+  </si>
+  <si>
+    <t>Rétrospective sprint 2</t>
+  </si>
+  <si>
+    <t>Preparation de l'envoi du mail</t>
+  </si>
+  <si>
+    <t>Rendu hebdomadaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise en page du word + journal de bord </t>
   </si>
 </sst>
 </file>
@@ -860,14 +905,14 @@
   </sheetPr>
   <dimension ref="B1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
     <col min="5" max="5" width="74" customWidth="1"/>
@@ -1290,65 +1335,137 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="18"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="20"/>
+    <row r="33" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="19">
+        <v>44327</v>
+      </c>
+      <c r="D33" s="20">
+        <v>30</v>
+      </c>
       <c r="E33" s="22"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="18"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="20"/>
+    <row r="34" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B34" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="19">
+        <v>44327</v>
+      </c>
+      <c r="D34" s="20">
+        <v>30</v>
+      </c>
       <c r="E34" s="22"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="18"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="22"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="22"/>
+    <row r="35" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B35" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="19">
+        <v>44327</v>
+      </c>
+      <c r="D35" s="20">
+        <v>15</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B36" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="19">
+        <v>44327</v>
+      </c>
+      <c r="D36" s="20">
+        <v>30</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="18"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="22"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="18"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="22"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="18"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="22"/>
+      <c r="B37" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="19">
+        <v>44327</v>
+      </c>
+      <c r="D37" s="20">
+        <v>60</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="19">
+        <v>44327</v>
+      </c>
+      <c r="D38" s="20">
+        <v>30</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B39" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="19">
+        <v>44327</v>
+      </c>
+      <c r="D39" s="20">
+        <v>120</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="7"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="9"/>
+      <c r="B40" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="19">
+        <v>44327</v>
+      </c>
+      <c r="D40" s="9">
+        <v>30</v>
+      </c>
       <c r="E40" s="22"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="7"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="22"/>
+      <c r="B41" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="19">
+        <v>44327</v>
+      </c>
+      <c r="D41" s="9">
+        <v>15</v>
+      </c>
+      <c r="E41" s="4"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="18"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="22"/>
+      <c r="B42" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="19">
+        <v>44327</v>
+      </c>
+      <c r="D42" s="9">
+        <v>15</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="18"/>

</xml_diff>

<commit_message>
Le login/register + template de calendrier
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord TPI.xlsx
+++ b/Documentation/Journal de bord TPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
   <si>
     <t>Date</t>
   </si>
@@ -231,6 +231,27 @@
   </si>
   <si>
     <t xml:space="preserve">Mise en page du word + journal de bord </t>
+  </si>
+  <si>
+    <t>Code du register</t>
+  </si>
+  <si>
+    <t>Ajustement visuel du register</t>
+  </si>
+  <si>
+    <t>Ajustement visuel du login</t>
+  </si>
+  <si>
+    <t>avec une case d'erreur si la connexion echoue</t>
+  </si>
+  <si>
+    <t>finission du login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout du calendrier trouver en exemple </t>
+  </si>
+  <si>
+    <t>en plus de tout les ajustement a faire des noms des variables du decorticage du php dans l'html, et de mettre le tout en structure MVC</t>
   </si>
 </sst>
 </file>
@@ -905,8 +926,8 @@
   </sheetPr>
   <dimension ref="B1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,34 +1489,70 @@
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="18"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="20"/>
+      <c r="B43" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" s="19">
+        <v>44333</v>
+      </c>
+      <c r="D43" s="20">
+        <v>60</v>
+      </c>
       <c r="E43" s="22"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="18"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="20"/>
+      <c r="B44" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" s="19">
+        <v>44333</v>
+      </c>
+      <c r="D44" s="20">
+        <v>120</v>
+      </c>
       <c r="E44" s="22"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="18"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="22"/>
+      <c r="B45" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" s="19">
+        <v>44333</v>
+      </c>
+      <c r="D45" s="20">
+        <v>60</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="18"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="22"/>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="18"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="22"/>
+      <c r="B46" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" s="19">
+        <v>44333</v>
+      </c>
+      <c r="D46" s="20">
+        <v>15</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B47" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47" s="19">
+        <v>44333</v>
+      </c>
+      <c r="D47" s="20">
+        <v>120</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="18"/>

</xml_diff>

<commit_message>
Mise en page de l'ajout d'un event + Surbrillance du jour sur le calendar
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord TPI.xlsx
+++ b/Documentation/Journal de bord TPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="90">
   <si>
     <t>Date</t>
   </si>
@@ -294,6 +294,12 @@
   </si>
   <si>
     <t>Creation de la bd sur swisscenter + update des fichiers du site</t>
+  </si>
+  <si>
+    <t>Ajout d'un evenement</t>
+  </si>
+  <si>
+    <t>Fonction d'ajout d'un evenement</t>
   </si>
 </sst>
 </file>
@@ -968,8 +974,8 @@
   </sheetPr>
   <dimension ref="B1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="B43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,10 +1731,18 @@
       <c r="E57" s="22"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="18"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="22"/>
+      <c r="B58" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" s="19">
+        <v>44336</v>
+      </c>
+      <c r="D58" s="20">
+        <v>120</v>
+      </c>
+      <c r="E58" s="22" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="18"/>

</xml_diff>

<commit_message>
AddAnEvent + update et delete pas encore en place
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord TPI.xlsx
+++ b/Documentation/Journal de bord TPI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13650" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10320" windowHeight="6840"/>
   </bookViews>
   <sheets>
     <sheet name="Page 1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
   <si>
     <t>Date</t>
   </si>
@@ -300,6 +300,33 @@
   </si>
   <si>
     <t>Fonction d'ajout d'un evenement</t>
+  </si>
+  <si>
+    <t>Visite du deuxieme expert</t>
+  </si>
+  <si>
+    <t>Reglage d'un bug sur le calendrier</t>
+  </si>
+  <si>
+    <t>Le jour d'aujourd'hui était en jaune meme au autre mois et année</t>
+  </si>
+  <si>
+    <t>Bug d'ajout d'un evenement</t>
+  </si>
+  <si>
+    <t>La query était juste mais ne marchait pas. Il a fallut des essais dans tout les sens pour voir que la copie de la BD s'etais mal faite et que l'ID était pas en auto incrementation</t>
+  </si>
+  <si>
+    <t>Creation de la fonction delete un event</t>
+  </si>
+  <si>
+    <t>Creation de la fonction update d'un event</t>
+  </si>
+  <si>
+    <t>Ajout d'une fonctionalité sur la gestion de date</t>
+  </si>
+  <si>
+    <t>Quand on clique pour gerer une date, si plusieurs evenement ont été ajouter, on peut tous les voir</t>
   </si>
 </sst>
 </file>
@@ -974,8 +1001,8 @@
   </sheetPr>
   <dimension ref="B1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="B46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,40 +1772,78 @@
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="18"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="22"/>
+      <c r="B59" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C59" s="19">
+        <v>44336</v>
+      </c>
+      <c r="D59" s="9">
+        <v>60</v>
+      </c>
+      <c r="E59" s="22" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="18"/>
-      <c r="C60" s="19"/>
-      <c r="D60" s="20"/>
+      <c r="B60" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" s="19">
+        <v>44336</v>
+      </c>
+      <c r="D60" s="20">
+        <v>30</v>
+      </c>
       <c r="E60" s="22"/>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="18"/>
-      <c r="C61" s="19"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="22"/>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="18"/>
-      <c r="C62" s="19"/>
-      <c r="D62" s="20"/>
+    <row r="61" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B61" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C61" s="19">
+        <v>44336</v>
+      </c>
+      <c r="D61" s="20">
+        <v>120</v>
+      </c>
+      <c r="E61" s="22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B62" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C62" s="19">
+        <v>44336</v>
+      </c>
+      <c r="D62" s="20">
+        <v>30</v>
+      </c>
       <c r="E62" s="22"/>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="18"/>
-      <c r="C63" s="19"/>
-      <c r="D63" s="20"/>
+    <row r="63" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B63" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C63" s="19">
+        <v>44336</v>
+      </c>
+      <c r="D63" s="20">
+        <v>60</v>
+      </c>
       <c r="E63" s="22"/>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="18"/>
+    <row r="64" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B64" s="18" t="s">
+        <v>97</v>
+      </c>
       <c r="C64" s="19"/>
       <c r="D64" s="20"/>
-      <c r="E64" s="22"/>
+      <c r="E64" s="22" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="18"/>

</xml_diff>

<commit_message>
ajouter / modifier un event fini supprimer en cours
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord TPI.xlsx
+++ b/Documentation/Journal de bord TPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="103">
   <si>
     <t>Date</t>
   </si>
@@ -327,6 +327,18 @@
   </si>
   <si>
     <t>Quand on clique pour gerer une date, si plusieurs evenement ont été ajouter, on peut tous les voir</t>
+  </si>
+  <si>
+    <t>Fonction modifier</t>
+  </si>
+  <si>
+    <t>Fonction supprimer</t>
+  </si>
+  <si>
+    <t>Mise a jour du site</t>
+  </si>
+  <si>
+    <t>En plus du mail de fin de semaine.</t>
   </si>
 </sst>
 </file>
@@ -1001,8 +1013,8 @@
   </sheetPr>
   <dimension ref="B1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,29 +1851,53 @@
       <c r="B64" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C64" s="19"/>
-      <c r="D64" s="20"/>
+      <c r="C64" s="19">
+        <v>44336</v>
+      </c>
+      <c r="D64" s="20">
+        <v>60</v>
+      </c>
       <c r="E64" s="22" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="18"/>
-      <c r="C65" s="19"/>
-      <c r="D65" s="20"/>
+      <c r="B65" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C65" s="19">
+        <v>44337</v>
+      </c>
+      <c r="D65" s="20">
+        <v>90</v>
+      </c>
       <c r="E65" s="22"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="18"/>
-      <c r="C66" s="19"/>
-      <c r="D66" s="20"/>
+      <c r="B66" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C66" s="19">
+        <v>44337</v>
+      </c>
+      <c r="D66" s="20">
+        <v>60</v>
+      </c>
       <c r="E66" s="22"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="18"/>
-      <c r="C67" s="19"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="22"/>
+      <c r="B67" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C67" s="19">
+        <v>44337</v>
+      </c>
+      <c r="D67" s="20">
+        <v>30</v>
+      </c>
+      <c r="E67" s="22" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="18"/>

</xml_diff>

<commit_message>
CRUD ended on the site.
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord TPI.xlsx
+++ b/Documentation/Journal de bord TPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="108">
   <si>
     <t>Date</t>
   </si>
@@ -339,6 +339,21 @@
   </si>
   <si>
     <t>En plus du mail de fin de semaine.</t>
+  </si>
+  <si>
+    <t>Reglage d'un bug de log in sur le server</t>
+  </si>
+  <si>
+    <t>Il était déjà present au moment du livrable</t>
+  </si>
+  <si>
+    <t>Buton supprimer a continuer de coder</t>
+  </si>
+  <si>
+    <t>Probleme de reperage entre la suppresion d'un event et l'update</t>
+  </si>
+  <si>
+    <t>J'ai du identifier les form individuellement avec des id et faire les redirections adequates.</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1029,7 @@
   <dimension ref="B1:E82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1899,23 +1914,45 @@
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="18"/>
-      <c r="C68" s="19"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="22"/>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="18"/>
-      <c r="C69" s="19"/>
-      <c r="D69" s="20"/>
+    <row r="68" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B68" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C68" s="19">
+        <v>44341</v>
+      </c>
+      <c r="D68" s="20">
+        <v>20</v>
+      </c>
+      <c r="E68" s="22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B69" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C69" s="19">
+        <v>44341</v>
+      </c>
+      <c r="D69" s="20">
+        <v>60</v>
+      </c>
       <c r="E69" s="22"/>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="18"/>
-      <c r="C70" s="19"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="22"/>
+    <row r="70" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B70" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C70" s="19">
+        <v>44341</v>
+      </c>
+      <c r="D70" s="20">
+        <v>60</v>
+      </c>
+      <c r="E70" s="22" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="18"/>

</xml_diff>

<commit_message>
Bouton sup added + popup bug regler + modifier fixed
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord TPI.xlsx
+++ b/Documentation/Journal de bord TPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="130">
   <si>
     <t>Date</t>
   </si>
@@ -416,6 +416,30 @@
   </si>
   <si>
     <t>Codage de l'affichage des reccurences</t>
+  </si>
+  <si>
+    <t>Sprint review 3</t>
+  </si>
+  <si>
+    <t>Sprint review avec le chef de projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correction d'un bug d'update d'event </t>
+  </si>
+  <si>
+    <t>Suite a la sprint review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correction d'un bug de delete d'event </t>
+  </si>
+  <si>
+    <t>Suite a la sprint review, ajout de la possibilité de pouvoir delete un event/une recurrence ou event + recurrence</t>
+  </si>
+  <si>
+    <t>Ajout d'un nombre de jour choisissable pour les recurrences</t>
+  </si>
+  <si>
+    <t>Ajout des jours de dates soulignées si nous avons un evenement ce jour</t>
   </si>
 </sst>
 </file>
@@ -458,7 +482,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -605,11 +629,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -660,6 +719,18 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -797,8 +868,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="B2:E81" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="B2:E81"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="B2:E100" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="B2:E100"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Tâche" dataDxfId="3"/>
     <tableColumn id="3" name="Date" dataDxfId="2"/>
@@ -1075,10 +1146,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:F86"/>
+  <dimension ref="B1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2134,41 +2205,170 @@
       <c r="E80" s="4"/>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B81" s="17"/>
-      <c r="C81" s="17"/>
-      <c r="D81" s="17"/>
-      <c r="E81" s="17"/>
+      <c r="B81" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="C81" s="15">
+        <v>44347</v>
+      </c>
+      <c r="D81" s="16">
+        <v>60</v>
+      </c>
+      <c r="E81" s="20" t="s">
+        <v>123</v>
+      </c>
       <c r="F81" s="17"/>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C82" s="17"/>
-      <c r="D82" s="17"/>
-      <c r="E82" s="17"/>
+      <c r="B82" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C82" s="15">
+        <v>44347</v>
+      </c>
+      <c r="D82" s="16">
+        <v>20</v>
+      </c>
+      <c r="E82" s="18" t="s">
+        <v>125</v>
+      </c>
       <c r="F82" s="17"/>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C83" s="17"/>
-      <c r="D83" s="17"/>
-      <c r="E83" s="17"/>
+    <row r="83" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B83" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C83" s="15">
+        <v>44347</v>
+      </c>
+      <c r="D83" s="16">
+        <v>120</v>
+      </c>
+      <c r="E83" s="18" t="s">
+        <v>127</v>
+      </c>
       <c r="F83" s="17"/>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C84" s="17"/>
-      <c r="D84" s="17"/>
-      <c r="E84" s="17"/>
+    <row r="84" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B84" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C84" s="15">
+        <v>44347</v>
+      </c>
+      <c r="D84" s="16">
+        <v>60</v>
+      </c>
+      <c r="E84" s="18" t="s">
+        <v>125</v>
+      </c>
       <c r="F84" s="17"/>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C85" s="17"/>
-      <c r="D85" s="17"/>
-      <c r="E85" s="17"/>
+    <row r="85" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B85" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C85" s="15">
+        <v>44347</v>
+      </c>
+      <c r="D85" s="16">
+        <v>120</v>
+      </c>
+      <c r="E85" s="18" t="s">
+        <v>125</v>
+      </c>
       <c r="F85" s="17"/>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C86" s="17"/>
-      <c r="D86" s="17"/>
-      <c r="E86" s="17"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="15"/>
+      <c r="D86" s="16"/>
+      <c r="E86" s="18"/>
       <c r="F86" s="17"/>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B87" s="14"/>
+      <c r="C87" s="15"/>
+      <c r="D87" s="16"/>
+      <c r="E87" s="18"/>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B88" s="14"/>
+      <c r="C88" s="15"/>
+      <c r="D88" s="16"/>
+      <c r="E88" s="18"/>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B89" s="14"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="16"/>
+      <c r="E89" s="18"/>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B90" s="14"/>
+      <c r="C90" s="15"/>
+      <c r="D90" s="16"/>
+      <c r="E90" s="18"/>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B91" s="14"/>
+      <c r="C91" s="15"/>
+      <c r="D91" s="16"/>
+      <c r="E91" s="18"/>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B92" s="14"/>
+      <c r="C92" s="15"/>
+      <c r="D92" s="16"/>
+      <c r="E92" s="18"/>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B93" s="14"/>
+      <c r="C93" s="15"/>
+      <c r="D93" s="16"/>
+      <c r="E93" s="18"/>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B94" s="14"/>
+      <c r="C94" s="15"/>
+      <c r="D94" s="16"/>
+      <c r="E94" s="18"/>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B95" s="14"/>
+      <c r="C95" s="15"/>
+      <c r="D95" s="16"/>
+      <c r="E95" s="18"/>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B96" s="14"/>
+      <c r="C96" s="15"/>
+      <c r="D96" s="16"/>
+      <c r="E96" s="18"/>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B97" s="14"/>
+      <c r="C97" s="15"/>
+      <c r="D97" s="16"/>
+      <c r="E97" s="18"/>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B98" s="14"/>
+      <c r="C98" s="15"/>
+      <c r="D98" s="16"/>
+      <c r="E98" s="18"/>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B99" s="14"/>
+      <c r="C99" s="15"/>
+      <c r="D99" s="16"/>
+      <c r="E99" s="18"/>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B100" s="22"/>
+      <c r="C100" s="23"/>
+      <c r="D100" s="16"/>
+      <c r="E100" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix bug popup + manuel d'installation / utilisation + documentation realisation
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord TPI.xlsx
+++ b/Documentation/Journal de bord TPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="135">
   <si>
     <t>Date</t>
   </si>
@@ -440,6 +440,21 @@
   </si>
   <si>
     <t>Ajout des jours de dates soulignées si nous avons un evenement ce jour</t>
+  </si>
+  <si>
+    <t>Partie 4 Realisation</t>
+  </si>
+  <si>
+    <t>Resumé du TPI</t>
+  </si>
+  <si>
+    <t>Creation du Manuel d'utilisation</t>
+  </si>
+  <si>
+    <t>Creation du Manuel d'installation</t>
+  </si>
+  <si>
+    <t>Fini</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1164,7 @@
   <dimension ref="B1:F100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2280,29 +2295,59 @@
       <c r="F85" s="17"/>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B86" s="14"/>
-      <c r="C86" s="15"/>
-      <c r="D86" s="16"/>
-      <c r="E86" s="18"/>
+      <c r="B86" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C86" s="15">
+        <v>44348</v>
+      </c>
+      <c r="D86" s="16">
+        <v>120</v>
+      </c>
+      <c r="E86" s="18" t="s">
+        <v>130</v>
+      </c>
       <c r="F86" s="17"/>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B87" s="14"/>
-      <c r="C87" s="15"/>
-      <c r="D87" s="16"/>
+      <c r="B87" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C87" s="15">
+        <v>44348</v>
+      </c>
+      <c r="D87" s="16">
+        <v>120</v>
+      </c>
       <c r="E87" s="18"/>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B88" s="14"/>
-      <c r="C88" s="15"/>
-      <c r="D88" s="16"/>
-      <c r="E88" s="18"/>
+      <c r="B88" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C88" s="15">
+        <v>44348</v>
+      </c>
+      <c r="D88" s="16">
+        <v>80</v>
+      </c>
+      <c r="E88" s="18" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B89" s="14"/>
-      <c r="C89" s="15"/>
-      <c r="D89" s="16"/>
-      <c r="E89" s="18"/>
+      <c r="B89" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C89" s="15">
+        <v>44348</v>
+      </c>
+      <c r="D89" s="16">
+        <v>60</v>
+      </c>
+      <c r="E89" s="18" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B90" s="14"/>

</xml_diff>

<commit_message>
Possible dernier push, check doc, dernier modfi code, PDF crée, Doxygen crée
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord TPI.xlsx
+++ b/Documentation/Journal de bord TPI.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="143">
   <si>
     <t>Date</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Ecriture du mail d'envoie des PDF</t>
   </si>
   <si>
-    <t>Cela m'a pris pas mal de temps, J'ai fais les maquettes pour l'acceuil, Mon calendrier vue mois et semaine, modifier/ajouter évènement, contact, login, register, profil</t>
-  </si>
-  <si>
     <t>Discussion avec le chef de projet</t>
   </si>
   <si>
@@ -185,30 +182,18 @@
     <t>Diagramme de code pour ajouter un évènement</t>
   </si>
   <si>
-    <t>Charte graphique + 2-3 autres points</t>
-  </si>
-  <si>
     <t>Diagramme de code pour modifier un évènement</t>
   </si>
   <si>
     <t>Diagramme de code pour supprimer un évènement</t>
   </si>
   <si>
-    <t>Modification de 2-3 trucs</t>
-  </si>
-  <si>
     <t>Reprise du debut de code du calendrier et mise a niveau des couleurs avec la charte graphique de la doc</t>
   </si>
   <si>
-    <t>Couleur + petite adaptation aux besoins</t>
-  </si>
-  <si>
     <t>Mise en place de l'hebergement</t>
   </si>
   <si>
-    <t>Discussion avec le chef de projet + ajout du site vitrine sur swisscenter</t>
-  </si>
-  <si>
     <t>Ajout des diagramme dans la documentation</t>
   </si>
   <si>
@@ -218,18 +203,12 @@
     <t>Pas encore au points a cause de tout ce qu'il faut retoucher. Ex: name des label du template, redirection, etc..</t>
   </si>
   <si>
-    <t>Sprint 2 fini a partir d'ici</t>
-  </si>
-  <si>
     <t>Rétrospective sprint 2</t>
   </si>
   <si>
     <t>Preparation de l'envoi du mail</t>
   </si>
   <si>
-    <t>Rendu hebdomadaire</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mise en page du word + journal de bord </t>
   </si>
   <si>
@@ -242,24 +221,15 @@
     <t>Ajustement visuel du login</t>
   </si>
   <si>
-    <t>avec une case d'erreur si la connexion echoue</t>
-  </si>
-  <si>
     <t>finission du login</t>
   </si>
   <si>
     <t xml:space="preserve">Ajout du calendrier trouver en exemple </t>
   </si>
   <si>
-    <t>en plus de tout les ajustement a faire des noms des variables du decorticage du php dans l'html, et de mettre le tout en structure MVC</t>
-  </si>
-  <si>
     <t>Aide apporté a un camarade</t>
   </si>
   <si>
-    <t>Jérôme jaquemet avait besoin d'aide pour l'élaboration des regles de sont TPI</t>
-  </si>
-  <si>
     <t xml:space="preserve">Decorticage en profondeur du code du calendrier </t>
   </si>
   <si>
@@ -272,18 +242,12 @@
     <t>Sprint 2 review</t>
   </si>
   <si>
-    <t>Avec le chef de projet</t>
-  </si>
-  <si>
     <t>Fonction du bouton aujourd'hui et fonctionel</t>
   </si>
   <si>
     <t>Ajout d'une fonction sur le calendrier</t>
   </si>
   <si>
-    <t>Quand il s'affiche, le jour d'aujourd'hui est d'une couleur differente</t>
-  </si>
-  <si>
     <t>Date du jour en surbrillance</t>
   </si>
   <si>
@@ -299,24 +263,15 @@
     <t>Ajout d'un evenement</t>
   </si>
   <si>
-    <t>Fonction d'ajout d'un evenement</t>
-  </si>
-  <si>
     <t>Visite du deuxieme expert</t>
   </si>
   <si>
     <t>Reglage d'un bug sur le calendrier</t>
   </si>
   <si>
-    <t>Le jour d'aujourd'hui était en jaune meme au autre mois et année</t>
-  </si>
-  <si>
     <t>Bug d'ajout d'un evenement</t>
   </si>
   <si>
-    <t>La query était juste mais ne marchait pas. Il a fallut des essais dans tout les sens pour voir que la copie de la BD s'etais mal faite et que l'ID était pas en auto incrementation</t>
-  </si>
-  <si>
     <t>Creation de la fonction delete un event</t>
   </si>
   <si>
@@ -326,9 +281,6 @@
     <t>Ajout d'une fonctionalité sur la gestion de date</t>
   </si>
   <si>
-    <t>Quand on clique pour gerer une date, si plusieurs evenement ont été ajouter, on peut tous les voir</t>
-  </si>
-  <si>
     <t>Fonction modifier</t>
   </si>
   <si>
@@ -342,9 +294,6 @@
   </si>
   <si>
     <t>Reglage d'un bug de log in sur le server</t>
-  </si>
-  <si>
-    <t>Il était déjà present au moment du livrable</t>
   </si>
   <si>
     <t>Buton supprimer a continuer de coder</t>
@@ -394,9 +343,6 @@
     <t>Update du git</t>
   </si>
   <si>
-    <t>ajout d'une release</t>
-  </si>
-  <si>
     <t>Ajout d'une future feature</t>
   </si>
   <si>
@@ -412,39 +358,24 @@
     <t>Codage de l'ajout d'une recurrence</t>
   </si>
   <si>
-    <t>Avant la recurence était afficher mais pas mis dans la table event-recurrence</t>
-  </si>
-  <si>
     <t>Codage de l'affichage des reccurences</t>
   </si>
   <si>
     <t>Sprint review 3</t>
   </si>
   <si>
-    <t>Sprint review avec le chef de projet</t>
-  </si>
-  <si>
     <t xml:space="preserve">Correction d'un bug d'update d'event </t>
   </si>
   <si>
-    <t>Suite a la sprint review</t>
-  </si>
-  <si>
     <t xml:space="preserve">Correction d'un bug de delete d'event </t>
   </si>
   <si>
-    <t>Suite a la sprint review, ajout de la possibilité de pouvoir delete un event/une recurrence ou event + recurrence</t>
-  </si>
-  <si>
     <t>Ajout d'un nombre de jour choisissable pour les recurrences</t>
   </si>
   <si>
     <t>Ajout des jours de dates soulignées si nous avons un evenement ce jour</t>
   </si>
   <si>
-    <t>Partie 4 Realisation</t>
-  </si>
-  <si>
     <t>Resumé du TPI</t>
   </si>
   <si>
@@ -454,7 +385,100 @@
     <t>Creation du Manuel d'installation</t>
   </si>
   <si>
-    <t>Fini</t>
+    <t>Documentation Doxygen</t>
+  </si>
+  <si>
+    <t>Generation du Doxygen + modification pour que cela aille en adequation avec mon projet.</t>
+  </si>
+  <si>
+    <t>Mise en page au propre de la documentation</t>
+  </si>
+  <si>
+    <t>Relecture des commentaires mis dans le code</t>
+  </si>
+  <si>
+    <t>Relecture en entier du code.</t>
+  </si>
+  <si>
+    <t>Finissage du point 4.</t>
+  </si>
+  <si>
+    <t>Fini.</t>
+  </si>
+  <si>
+    <t>Partie 4 Realisation.</t>
+  </si>
+  <si>
+    <t>Suite a la sprint review.</t>
+  </si>
+  <si>
+    <t>Suite a la sprint review, ajout de la possibilité de pouvoir delete un event/une recurrence ou event + recurrence.</t>
+  </si>
+  <si>
+    <t>Sprint review avec le chef de projet.</t>
+  </si>
+  <si>
+    <t>Avant la recurence était afficher mais pas mis dans la table event-recurrence.</t>
+  </si>
+  <si>
+    <t>Ajout d'une release.</t>
+  </si>
+  <si>
+    <t>Il était déjà present au moment du livrable.</t>
+  </si>
+  <si>
+    <t>Quand on clique pour gerer une date, si plusieurs evenement ont été ajouter, on peut tous les voir.</t>
+  </si>
+  <si>
+    <t>La query était juste mais ne marchait pas. Il a fallut des essais dans tout les sens pour voir que la copie de la BD s'etais mal faite et que l'ID était pas en auto incrementation.</t>
+  </si>
+  <si>
+    <t>Le jour d'aujourd'hui était en jaune meme au autre mois et année.</t>
+  </si>
+  <si>
+    <t>Fonction d'ajout d'un evenement.</t>
+  </si>
+  <si>
+    <t>Quand il s'affiche, le jour d'aujourd'hui est d'une couleur differente.</t>
+  </si>
+  <si>
+    <t>Avec le chef de projet.</t>
+  </si>
+  <si>
+    <t>Jérôme jaquemet avait besoin d'aide pour l'élaboration des regles de sont TPI.</t>
+  </si>
+  <si>
+    <t>en plus de tout les ajustement a faire des noms des variables du decorticage du php dans l'html, et de mettre le tout en structure MVC.</t>
+  </si>
+  <si>
+    <t>Avec une case d'erreur si la connexion echoue.</t>
+  </si>
+  <si>
+    <t>Rendu hebdomadaire.</t>
+  </si>
+  <si>
+    <t>Sprint 2 fini a partir d'ici.</t>
+  </si>
+  <si>
+    <t>Discussion avec le chef de projet + ajout du site vitrine sur swisscenter.</t>
+  </si>
+  <si>
+    <t>Couleur + petite adaptation aux besoins.</t>
+  </si>
+  <si>
+    <t>Modification de 2-3 trucs.</t>
+  </si>
+  <si>
+    <t>Charte graphique + 2-3 autres points.</t>
+  </si>
+  <si>
+    <t>Cela m'a pris pas mal de temps, J'ai fais les maquettes pour l'acceuil, Mon calendrier vue mois et semaine, modifier/ajouter évènement, contact, login, register, profil.</t>
+  </si>
+  <si>
+    <t>Ecriture du mail d'envoie final</t>
+  </si>
+  <si>
+    <t>Correction d'un bug d'affichage uniquement present sur le server</t>
   </si>
 </sst>
 </file>
@@ -1163,8 +1187,8 @@
   </sheetPr>
   <dimension ref="B1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,7 +1228,7 @@
         <v>45</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -1218,7 +1242,7 @@
         <v>45</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -1244,7 +1268,7 @@
         <v>120</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -1258,7 +1282,7 @@
         <v>60</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
@@ -1320,7 +1344,7 @@
         <v>120</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -1346,7 +1370,7 @@
         <v>120</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -1360,7 +1384,7 @@
         <v>40</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1374,7 +1398,7 @@
         <v>15</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="45" x14ac:dyDescent="0.25">
@@ -1388,12 +1412,12 @@
         <v>180</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>19</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="8">
         <v>44322</v>
@@ -1402,12 +1426,12 @@
         <v>10</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="8">
         <v>44322</v>
@@ -1428,12 +1452,12 @@
         <v>120</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="8">
         <v>44322</v>
@@ -1442,12 +1466,12 @@
         <v>60</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="8">
         <v>44323</v>
@@ -1456,12 +1480,12 @@
         <v>60</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="8">
         <v>44323</v>
@@ -1470,12 +1494,12 @@
         <v>30</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="8">
         <v>44323</v>
@@ -1484,12 +1508,12 @@
         <v>60</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B25" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="8">
         <v>44323</v>
@@ -1498,12 +1522,12 @@
         <v>60</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" s="8">
         <v>44326</v>
@@ -1515,7 +1539,7 @@
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" s="8">
         <v>44326</v>
@@ -1527,7 +1551,7 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" s="8">
         <v>44326</v>
@@ -1536,12 +1560,12 @@
         <v>30</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="8">
         <v>44326</v>
@@ -1550,12 +1574,12 @@
         <v>60</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" s="8">
         <v>44326</v>
@@ -1564,12 +1588,12 @@
         <v>120</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C31" s="8">
         <v>44326</v>
@@ -1590,12 +1614,12 @@
         <v>30</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>51</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C33" s="15">
         <v>44327</v>
@@ -1607,7 +1631,7 @@
     </row>
     <row r="34" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C34" s="15">
         <v>44327</v>
@@ -1619,7 +1643,7 @@
     </row>
     <row r="35" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C35" s="15">
         <v>44327</v>
@@ -1628,12 +1652,12 @@
         <v>15</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>54</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B36" s="14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C36" s="15">
         <v>44327</v>
@@ -1642,12 +1666,12 @@
         <v>30</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>56</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C37" s="15">
         <v>44327</v>
@@ -1656,12 +1680,12 @@
         <v>60</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>58</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="14" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C38" s="15">
         <v>44327</v>
@@ -1670,12 +1694,12 @@
         <v>30</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>62</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="14" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C39" s="15">
         <v>44327</v>
@@ -1684,12 +1708,12 @@
         <v>120</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C40" s="15">
         <v>44327</v>
@@ -1701,7 +1725,7 @@
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="7" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C41" s="15">
         <v>44327</v>
@@ -1713,7 +1737,7 @@
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C42" s="15">
         <v>44327</v>
@@ -1722,12 +1746,12 @@
         <v>15</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>65</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="14" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C43" s="15">
         <v>44333</v>
@@ -1739,7 +1763,7 @@
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="14" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C44" s="15">
         <v>44333</v>
@@ -1751,7 +1775,7 @@
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="14" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C45" s="15">
         <v>44333</v>
@@ -1760,12 +1784,12 @@
         <v>60</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="14" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C46" s="15">
         <v>44333</v>
@@ -1774,12 +1798,12 @@
         <v>15</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="14" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C47" s="15">
         <v>44333</v>
@@ -1788,12 +1812,12 @@
         <v>120</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="14" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C48" s="15">
         <v>44333</v>
@@ -1805,7 +1829,7 @@
     </row>
     <row r="49" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B49" s="14" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C49" s="15">
         <v>44333</v>
@@ -1817,7 +1841,7 @@
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="14" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C50" s="15">
         <v>44333</v>
@@ -1826,12 +1850,12 @@
         <v>10</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>75</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B51" s="14" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C51" s="15">
         <v>44334</v>
@@ -1843,7 +1867,7 @@
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="14" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C52" s="15">
         <v>44334</v>
@@ -1852,12 +1876,12 @@
         <v>30</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>80</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B53" s="14" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C53" s="15">
         <v>44334</v>
@@ -1869,7 +1893,7 @@
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="14" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C54" s="15">
         <v>44334</v>
@@ -1878,12 +1902,12 @@
         <v>60</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>83</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="14" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C55" s="15">
         <v>44334</v>
@@ -1895,7 +1919,7 @@
     </row>
     <row r="56" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B56" s="14" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C56" s="15">
         <v>44334</v>
@@ -1904,12 +1928,12 @@
         <v>60</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B57" s="14" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C57" s="15">
         <v>44334</v>
@@ -1921,7 +1945,7 @@
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="14" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C58" s="15">
         <v>44336</v>
@@ -1930,12 +1954,12 @@
         <v>120</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>89</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C59" s="15">
         <v>44336</v>
@@ -1944,12 +1968,12 @@
         <v>60</v>
       </c>
       <c r="E59" s="18" t="s">
-        <v>92</v>
+        <v>127</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="14" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C60" s="15">
         <v>44336</v>
@@ -1961,7 +1985,7 @@
     </row>
     <row r="61" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B61" s="14" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C61" s="15">
         <v>44336</v>
@@ -1970,12 +1994,12 @@
         <v>120</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B62" s="14" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="C62" s="15">
         <v>44336</v>
@@ -1987,7 +2011,7 @@
     </row>
     <row r="63" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="14" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="C63" s="15">
         <v>44336</v>
@@ -1999,7 +2023,7 @@
     </row>
     <row r="64" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B64" s="14" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="C64" s="15">
         <v>44336</v>
@@ -2008,12 +2032,12 @@
         <v>60</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="14" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C65" s="15">
         <v>44337</v>
@@ -2025,7 +2049,7 @@
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="14" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C66" s="15">
         <v>44337</v>
@@ -2037,7 +2061,7 @@
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="14" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="C67" s="15">
         <v>44337</v>
@@ -2046,12 +2070,12 @@
         <v>30</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B68" s="14" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="C68" s="15">
         <v>44341</v>
@@ -2060,12 +2084,12 @@
         <v>20</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
     </row>
     <row r="69" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B69" s="14" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="C69" s="15">
         <v>44341</v>
@@ -2077,7 +2101,7 @@
     </row>
     <row r="70" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B70" s="14" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C70" s="15">
         <v>44341</v>
@@ -2086,12 +2110,12 @@
         <v>60</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="7" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="C71" s="15">
         <v>44341</v>
@@ -2100,12 +2124,12 @@
         <v>60</v>
       </c>
       <c r="E71" s="18" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="72" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B72" s="14" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="C72" s="15">
         <v>44341</v>
@@ -2117,7 +2141,7 @@
     </row>
     <row r="73" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B73" s="14" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="C73" s="15">
         <v>44341</v>
@@ -2126,7 +2150,7 @@
         <v>60</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
@@ -2143,7 +2167,7 @@
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" s="14" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="C75" s="15">
         <v>44341</v>
@@ -2152,12 +2176,12 @@
         <v>20</v>
       </c>
       <c r="E75" s="18" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="14" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="C76" s="15">
         <v>44341</v>
@@ -2166,12 +2190,12 @@
         <v>30</v>
       </c>
       <c r="E76" s="18" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
     </row>
     <row r="77" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B77" s="14" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="C77" s="15">
         <v>44343</v>
@@ -2183,7 +2207,7 @@
     </row>
     <row r="78" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B78" s="14" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="C78" s="15">
         <v>44343</v>
@@ -2195,7 +2219,7 @@
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79" s="14" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="C79" s="15">
         <v>44344</v>
@@ -2204,12 +2228,12 @@
         <v>120</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="80" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B80" s="14" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="C80" s="15">
         <v>44344</v>
@@ -2221,7 +2245,7 @@
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81" s="20" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="C81" s="15">
         <v>44347</v>
@@ -2230,13 +2254,13 @@
         <v>60</v>
       </c>
       <c r="E81" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F81" s="17"/>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" s="14" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C82" s="15">
         <v>44347</v>
@@ -2245,13 +2269,13 @@
         <v>20</v>
       </c>
       <c r="E82" s="18" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F82" s="17"/>
     </row>
     <row r="83" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B83" s="14" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="C83" s="15">
         <v>44347</v>
@@ -2260,13 +2284,13 @@
         <v>120</v>
       </c>
       <c r="E83" s="18" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F83" s="17"/>
     </row>
     <row r="84" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B84" s="14" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="C84" s="15">
         <v>44347</v>
@@ -2275,13 +2299,13 @@
         <v>60</v>
       </c>
       <c r="E84" s="18" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F84" s="17"/>
     </row>
     <row r="85" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B85" s="14" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="C85" s="15">
         <v>44347</v>
@@ -2290,7 +2314,7 @@
         <v>120</v>
       </c>
       <c r="E85" s="18" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F85" s="17"/>
     </row>
@@ -2305,13 +2329,13 @@
         <v>120</v>
       </c>
       <c r="E86" s="18" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="F86" s="17"/>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87" s="14" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="C87" s="15">
         <v>44348</v>
@@ -2323,7 +2347,7 @@
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B88" s="14" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="C88" s="15">
         <v>44348</v>
@@ -2332,12 +2356,12 @@
         <v>80</v>
       </c>
       <c r="E88" s="18" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B89" s="14" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="C89" s="15">
         <v>44348</v>
@@ -2346,43 +2370,85 @@
         <v>60</v>
       </c>
       <c r="E89" s="18" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B90" s="14"/>
-      <c r="C90" s="15"/>
-      <c r="D90" s="16"/>
-      <c r="E90" s="18"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B90" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C90" s="15">
+        <v>44350</v>
+      </c>
+      <c r="D90" s="16">
+        <v>60</v>
+      </c>
+      <c r="E90" s="18" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B91" s="14"/>
-      <c r="C91" s="15"/>
-      <c r="D91" s="16"/>
-      <c r="E91" s="18"/>
-    </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B92" s="14"/>
-      <c r="C92" s="15"/>
-      <c r="D92" s="16"/>
-      <c r="E92" s="18"/>
-    </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B93" s="14"/>
-      <c r="C93" s="15"/>
-      <c r="D93" s="16"/>
+      <c r="B91" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C91" s="15">
+        <v>44350</v>
+      </c>
+      <c r="D91" s="16">
+        <v>120</v>
+      </c>
+      <c r="E91" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B92" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C92" s="15">
+        <v>44350</v>
+      </c>
+      <c r="D92" s="16">
+        <v>120</v>
+      </c>
+      <c r="E92" s="18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B93" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C93" s="15">
+        <v>44350</v>
+      </c>
+      <c r="D93" s="16">
+        <v>60</v>
+      </c>
       <c r="E93" s="18"/>
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B94" s="14"/>
-      <c r="C94" s="15"/>
-      <c r="D94" s="16"/>
+      <c r="B94" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C94" s="15">
+        <v>44350</v>
+      </c>
+      <c r="D94" s="16">
+        <v>60</v>
+      </c>
       <c r="E94" s="18"/>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B95" s="14"/>
-      <c r="C95" s="15"/>
-      <c r="D95" s="16"/>
+    <row r="95" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B95" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C95" s="15">
+        <v>44350</v>
+      </c>
+      <c r="D95" s="16">
+        <v>60</v>
+      </c>
       <c r="E95" s="18"/>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>